<commit_message>
Deploying to gh-pages from @ koodiklinikka/palkkakysely@389ee524fbca235e9f3a4440f144846bde95f107 🚀
</commit_message>
<xml_diff>
--- a/raw.xlsx
+++ b/raw.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2926" uniqueCount="404">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2967" uniqueCount="409">
   <si>
     <t>Timestamp</t>
   </si>
@@ -1223,6 +1223,21 @@
   </si>
   <si>
     <t>Optiot</t>
+  </si>
+  <si>
+    <t>Full-stack ohjelmistokehittäjä (junior)</t>
+  </si>
+  <si>
+    <t>ATR Soft</t>
+  </si>
+  <si>
+    <t>Viimsi</t>
+  </si>
+  <si>
+    <t>sysadmin</t>
+  </si>
+  <si>
+    <t>Ohjelmistosuunnittelija</t>
   </si>
 </sst>
 </file>
@@ -16792,6 +16807,225 @@
         <v>27</v>
       </c>
     </row>
+    <row r="407">
+      <c r="A407" s="3">
+        <v>44246.611578344906</v>
+      </c>
+      <c r="B407" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C407" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D407" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E407" s="2">
+        <v>7.0</v>
+      </c>
+      <c r="F407" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G407" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="H407" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="I407" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J407" s="2">
+        <v>3900.0</v>
+      </c>
+      <c r="K407" s="2">
+        <v>55000.0</v>
+      </c>
+      <c r="L407" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" s="3">
+        <v>44246.61251465278</v>
+      </c>
+      <c r="B408" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C408" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D408" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E408" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="F408" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G408" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="H408" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="I408" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="J408" s="2">
+        <v>3200.0</v>
+      </c>
+      <c r="K408" s="2">
+        <v>40000.0</v>
+      </c>
+      <c r="L408" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" s="3">
+        <v>44246.613068645835</v>
+      </c>
+      <c r="B409" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C409" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D409" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E409" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="F409" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G409" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="H409" s="2" t="s">
+        <v>404</v>
+      </c>
+      <c r="I409" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J409" s="2">
+        <v>2600.0</v>
+      </c>
+      <c r="K409" s="2">
+        <v>32500.0</v>
+      </c>
+      <c r="L409" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="M409" s="2" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" s="3">
+        <v>44246.61409989583</v>
+      </c>
+      <c r="B410" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C410" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E410" s="2">
+        <v>5.0</v>
+      </c>
+      <c r="F410" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G410" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="H410" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I410" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J410" s="2">
+        <v>2900.0</v>
+      </c>
+      <c r="K410" s="2">
+        <v>36000.0</v>
+      </c>
+      <c r="L410" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" s="3">
+        <v>44246.61679134259</v>
+      </c>
+      <c r="B411" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="C411" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D411" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E411" s="2">
+        <v>20.0</v>
+      </c>
+      <c r="F411" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H411" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="I411" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K411" s="2">
+        <v>110000.0</v>
+      </c>
+      <c r="L411" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" s="3">
+        <v>44246.62107894676</v>
+      </c>
+      <c r="B412" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C412" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E412" s="2">
+        <v>12.0</v>
+      </c>
+      <c r="F412" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G412" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="H412" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="I412" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="J412" s="2">
+        <v>3800.0</v>
+      </c>
+      <c r="K412" s="2">
+        <v>50000.0</v>
+      </c>
+      <c r="L412" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ koodiklinikka/palkkakysely@ce51a4625a77ba24ad72d6823a96bd4594802e22 🚀
</commit_message>
<xml_diff>
--- a/raw.xlsx
+++ b/raw.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3103" uniqueCount="428">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3118" uniqueCount="429">
   <si>
     <t>Timestamp</t>
   </si>
@@ -1295,6 +1295,9 @@
   </si>
   <si>
     <t>Frontend ohjelmistokehittäjä</t>
+  </si>
+  <si>
+    <t>Tekninen asiantuntija/suunnittelija</t>
   </si>
 </sst>
 </file>
@@ -17788,6 +17791,85 @@
         <v>19</v>
       </c>
     </row>
+    <row r="431">
+      <c r="A431" s="3">
+        <v>44246.76441186343</v>
+      </c>
+      <c r="B431" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C431" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D431" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E431" s="2">
+        <v>6.0</v>
+      </c>
+      <c r="F431" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G431" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="H431" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="I431" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J431" s="2">
+        <v>3250.0</v>
+      </c>
+      <c r="K431" s="2">
+        <v>42000.0</v>
+      </c>
+      <c r="L431" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" s="3">
+        <v>44246.77388896991</v>
+      </c>
+      <c r="B432" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C432" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D432" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E432" s="2">
+        <v>12.0</v>
+      </c>
+      <c r="F432" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G432" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="H432" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I432" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J432" s="2">
+        <v>3000.0</v>
+      </c>
+      <c r="K432" s="2">
+        <v>37500.0</v>
+      </c>
+      <c r="L432" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="M432" s="2" t="s">
+        <v>305</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ koodiklinikka/palkkakysely@9572fbc0e20e99c6cd53b85a2080ca9904ea3c33 🚀
</commit_message>
<xml_diff>
--- a/raw.xlsx
+++ b/raw.xlsx
@@ -1488,10 +1488,12 @@
       <sz val="10.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <color theme="1"/>
       <name val="Arial"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -4303,9 +4305,9 @@
       <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="20" width="21.57"/>
+    <col customWidth="1" min="1" max="20" width="18.88"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -23249,7 +23251,7 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1"/>
     <row r="2"/>

</xml_diff>